<commit_message>
Added the missing row for wednesday
</commit_message>
<xml_diff>
--- a/CS297_TimeTracking.xlsx
+++ b/CS297_TimeTracking.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DataCard/Repos/CS297-CourseMaterials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47C3D842-AE65-BB4D-9628-B0FF5862F40A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9DAADF2-EC61-0148-AC2A-732001394793}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14800" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14800" tabRatio="500" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Totals" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="29">
   <si>
     <t>Week 1</t>
   </si>
@@ -119,6 +119,12 @@
   </si>
   <si>
     <t>Members:</t>
+  </si>
+  <si>
+    <t>Wednesday</t>
+  </si>
+  <si>
+    <t>`</t>
   </si>
 </sst>
 </file>
@@ -443,8 +449,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView zoomScale="200" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -503,7 +509,7 @@
         <v>0</v>
       </c>
       <c r="B4">
-        <f>'Week 1'!C$9</f>
+        <f>'Week 1'!C$10</f>
         <v>0</v>
       </c>
       <c r="C4">
@@ -511,7 +517,7 @@
         <v>0</v>
       </c>
       <c r="D4">
-        <f>'Week 1'!E$9</f>
+        <f>'Week 1'!E$10</f>
         <v>0</v>
       </c>
       <c r="E4">
@@ -519,7 +525,7 @@
         <v>0</v>
       </c>
       <c r="F4">
-        <f>'Week 1'!G$9</f>
+        <f>'Week 1'!G$10</f>
         <v>0</v>
       </c>
       <c r="G4">
@@ -527,7 +533,7 @@
         <v>0</v>
       </c>
       <c r="H4">
-        <f>'Week 1'!I$9</f>
+        <f>'Week 1'!I$10</f>
         <v>0</v>
       </c>
       <c r="I4">
@@ -540,7 +546,7 @@
         <v>1</v>
       </c>
       <c r="B5">
-        <f>'Week 2'!C$9</f>
+        <f>'Week 2'!C$10</f>
         <v>0</v>
       </c>
       <c r="C5">
@@ -548,7 +554,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <f>'Week 2'!E$9</f>
+        <f>'Week 2'!E$10</f>
         <v>0</v>
       </c>
       <c r="E5">
@@ -556,7 +562,7 @@
         <v>0</v>
       </c>
       <c r="F5">
-        <f>'Week 2'!G$9</f>
+        <f>'Week 2'!G$10</f>
         <v>0</v>
       </c>
       <c r="G5">
@@ -564,7 +570,7 @@
         <v>0</v>
       </c>
       <c r="H5">
-        <f>'Week 2'!I$9</f>
+        <f>'Week 2'!I$10</f>
         <v>0</v>
       </c>
       <c r="I5">
@@ -577,7 +583,7 @@
         <v>2</v>
       </c>
       <c r="B6">
-        <f>'Week 3'!C$9</f>
+        <f>'Week 3'!C$10</f>
         <v>0</v>
       </c>
       <c r="C6">
@@ -585,7 +591,7 @@
         <v>0</v>
       </c>
       <c r="D6">
-        <f>'Week 3'!E$9</f>
+        <f>'Week 3'!E$10</f>
         <v>0</v>
       </c>
       <c r="E6">
@@ -593,7 +599,7 @@
         <v>0</v>
       </c>
       <c r="F6">
-        <f>'Week 3'!G$9</f>
+        <f>'Week 3'!G$10</f>
         <v>0</v>
       </c>
       <c r="G6">
@@ -601,7 +607,7 @@
         <v>0</v>
       </c>
       <c r="H6">
-        <f>'Week 3'!I$9</f>
+        <f>'Week 3'!I$10</f>
         <v>0</v>
       </c>
       <c r="I6">
@@ -614,7 +620,7 @@
         <v>3</v>
       </c>
       <c r="B7">
-        <f>'Week 4'!C$9</f>
+        <f>'Week 4'!C$10</f>
         <v>0</v>
       </c>
       <c r="C7">
@@ -622,7 +628,7 @@
         <v>0</v>
       </c>
       <c r="D7">
-        <f>'Week 4'!E$9</f>
+        <f>'Week 4'!E$10</f>
         <v>0</v>
       </c>
       <c r="E7">
@@ -630,7 +636,7 @@
         <v>0</v>
       </c>
       <c r="F7">
-        <f>'Week 4'!G$9</f>
+        <f>'Week 4'!G$10</f>
         <v>0</v>
       </c>
       <c r="G7">
@@ -638,7 +644,7 @@
         <v>0</v>
       </c>
       <c r="H7">
-        <f>'Week 4'!I$9</f>
+        <f>'Week 4'!I$10</f>
         <v>0</v>
       </c>
       <c r="I7">
@@ -651,7 +657,7 @@
         <v>4</v>
       </c>
       <c r="B8">
-        <f>'Week 5'!C$9</f>
+        <f>'Week 5'!C$10</f>
         <v>0</v>
       </c>
       <c r="C8">
@@ -659,7 +665,7 @@
         <v>0</v>
       </c>
       <c r="D8">
-        <f>'Week 5'!E$9</f>
+        <f>'Week 5'!E$10</f>
         <v>0</v>
       </c>
       <c r="E8">
@@ -667,7 +673,7 @@
         <v>0</v>
       </c>
       <c r="F8">
-        <f>'Week 5'!G$9</f>
+        <f>'Week 5'!G$10</f>
         <v>0</v>
       </c>
       <c r="G8">
@@ -675,7 +681,7 @@
         <v>0</v>
       </c>
       <c r="H8">
-        <f>'Week 5'!I$9</f>
+        <f>'Week 5'!I$10</f>
         <v>0</v>
       </c>
       <c r="I8">
@@ -688,7 +694,7 @@
         <v>5</v>
       </c>
       <c r="B9">
-        <f>'Week 6'!C$9</f>
+        <f>'Week 6'!C$10</f>
         <v>0</v>
       </c>
       <c r="C9">
@@ -696,7 +702,7 @@
         <v>0</v>
       </c>
       <c r="D9">
-        <f>'Week 6'!E$9</f>
+        <f>'Week 6'!E$10</f>
         <v>0</v>
       </c>
       <c r="E9">
@@ -704,7 +710,7 @@
         <v>0</v>
       </c>
       <c r="F9">
-        <f>'Week 6'!G$9</f>
+        <f>'Week 6'!G$10</f>
         <v>0</v>
       </c>
       <c r="G9">
@@ -712,7 +718,7 @@
         <v>0</v>
       </c>
       <c r="H9">
-        <f>'Week 6'!I$9</f>
+        <f>'Week 6'!I$10</f>
         <v>0</v>
       </c>
       <c r="I9">
@@ -725,7 +731,7 @@
         <v>6</v>
       </c>
       <c r="B10">
-        <f>'Week 7'!C$9</f>
+        <f>'Week 7'!C$10</f>
         <v>0</v>
       </c>
       <c r="C10">
@@ -733,7 +739,7 @@
         <v>0</v>
       </c>
       <c r="D10">
-        <f>'Week 7'!E$9</f>
+        <f>'Week 7'!E$10</f>
         <v>0</v>
       </c>
       <c r="E10">
@@ -741,7 +747,7 @@
         <v>0</v>
       </c>
       <c r="F10">
-        <f>'Week 7'!G$9</f>
+        <f>'Week 7'!G$10</f>
         <v>0</v>
       </c>
       <c r="G10">
@@ -749,7 +755,7 @@
         <v>0</v>
       </c>
       <c r="H10">
-        <f>'Week 7'!I$9</f>
+        <f>'Week 7'!I$10</f>
         <v>0</v>
       </c>
       <c r="I10">
@@ -762,7 +768,7 @@
         <v>7</v>
       </c>
       <c r="B11">
-        <f>'Week 8'!C$9</f>
+        <f>'Week 8'!C$10</f>
         <v>0</v>
       </c>
       <c r="C11">
@@ -770,7 +776,7 @@
         <v>0</v>
       </c>
       <c r="D11">
-        <f>'Week 8'!E$9</f>
+        <f>'Week 8'!E$10</f>
         <v>0</v>
       </c>
       <c r="E11">
@@ -778,7 +784,7 @@
         <v>0</v>
       </c>
       <c r="F11">
-        <f>'Week 8'!G$9</f>
+        <f>'Week 8'!G$10</f>
         <v>0</v>
       </c>
       <c r="G11">
@@ -786,7 +792,7 @@
         <v>0</v>
       </c>
       <c r="H11">
-        <f>'Week 8'!I$9</f>
+        <f>'Week 8'!I$10</f>
         <v>0</v>
       </c>
       <c r="I11">
@@ -799,7 +805,7 @@
         <v>8</v>
       </c>
       <c r="B12">
-        <f>'Week 9'!C$9</f>
+        <f>'Week 9'!C$10</f>
         <v>0</v>
       </c>
       <c r="C12">
@@ -807,7 +813,7 @@
         <v>0</v>
       </c>
       <c r="D12">
-        <f>'Week 9'!E$9</f>
+        <f>'Week 9'!E$10</f>
         <v>0</v>
       </c>
       <c r="E12">
@@ -815,7 +821,7 @@
         <v>0</v>
       </c>
       <c r="F12">
-        <f>'Week 9'!G$9</f>
+        <f>'Week 9'!G$10</f>
         <v>0</v>
       </c>
       <c r="G12">
@@ -823,7 +829,7 @@
         <v>0</v>
       </c>
       <c r="H12">
-        <f>'Week 9'!I$9</f>
+        <f>'Week 9'!I$10</f>
         <v>0</v>
       </c>
       <c r="I12">
@@ -836,7 +842,7 @@
         <v>9</v>
       </c>
       <c r="B13">
-        <f>'Week 10'!C$9</f>
+        <f>'Week 10'!C$10</f>
         <v>0</v>
       </c>
       <c r="C13">
@@ -844,7 +850,7 @@
         <v>0</v>
       </c>
       <c r="D13">
-        <f>'Week 10'!E$9</f>
+        <f>'Week 10'!E$10</f>
         <v>0</v>
       </c>
       <c r="E13">
@@ -852,7 +858,7 @@
         <v>0</v>
       </c>
       <c r="F13">
-        <f>'Week 10'!G$9</f>
+        <f>'Week 10'!G$10</f>
         <v>0</v>
       </c>
       <c r="G13">
@@ -860,7 +866,7 @@
         <v>0</v>
       </c>
       <c r="H13">
-        <f>'Week 10'!I$9</f>
+        <f>'Week 10'!I$10</f>
         <v>0</v>
       </c>
       <c r="I13">
@@ -886,10 +892,10 @@
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4664E869-4EFD-D049-B01D-CBB6D687D0CE}">
   <sheetPr codeName="Sheet11"/>
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView zoomScale="200" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="A6" sqref="A6:I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1002,61 +1008,61 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6">
-        <f t="shared" ref="C6:I9" si="0">B6+C5</f>
+        <f>B6+C5</f>
         <v>0</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6">
-        <f t="shared" si="0"/>
+        <f>D6+E5</f>
         <v>0</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6">
-        <f t="shared" si="0"/>
+        <f>F6+G5</f>
         <v>0</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6">
-        <f t="shared" si="0"/>
+        <f>H6+I5</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7">
-        <f t="shared" si="0"/>
+        <f>B7+C6</f>
         <v>0</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7">
-        <f t="shared" si="0"/>
+        <f>D7+E6</f>
         <v>0</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7">
-        <f t="shared" si="0"/>
+        <f>F7+G6</f>
         <v>0</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7">
-        <f t="shared" si="0"/>
+        <f>H7+I6</f>
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="C8:I10" si="0">B8+C7</f>
         <v>0</v>
       </c>
       <c r="D8" s="1"/>
@@ -1077,7 +1083,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9">
@@ -1100,8 +1106,33 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F10" s="1"/>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H10" s="1"/>
+      <c r="I10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1114,10 +1145,10 @@
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{302849AC-C4A6-8D4B-9A02-FE599868F019}">
   <sheetPr codeName="Sheet12"/>
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView zoomScale="200" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" zoomScale="200" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1230,61 +1261,61 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6">
-        <f t="shared" ref="C6:I9" si="0">B6+C5</f>
+        <f>B6+C5</f>
         <v>0</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6">
-        <f t="shared" si="0"/>
+        <f>D6+E5</f>
         <v>0</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6">
-        <f t="shared" si="0"/>
+        <f>F6+G5</f>
         <v>0</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6">
-        <f t="shared" si="0"/>
+        <f>H6+I5</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7">
-        <f t="shared" si="0"/>
+        <f>B7+C6</f>
         <v>0</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7">
-        <f t="shared" si="0"/>
+        <f>D7+E6</f>
         <v>0</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7">
-        <f t="shared" si="0"/>
+        <f>F7+G6</f>
         <v>0</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7">
-        <f t="shared" si="0"/>
+        <f>H7+I6</f>
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="C8:I10" si="0">B8+C7</f>
         <v>0</v>
       </c>
       <c r="D8" s="1"/>
@@ -1305,7 +1336,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9">
@@ -1328,8 +1359,33 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F10" s="1"/>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H10" s="1"/>
+      <c r="I10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1342,10 +1398,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC11E001-DA2D-DB40-B076-5732B774C833}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView zoomScale="200" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:B9"/>
+      <selection activeCell="A6" sqref="A6:I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1458,61 +1514,61 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6">
-        <f t="shared" ref="C6:I9" si="0">B6+C5</f>
+        <f>B6+C5</f>
         <v>0</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6">
-        <f t="shared" si="0"/>
+        <f>D6+E5</f>
         <v>0</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6">
-        <f t="shared" si="0"/>
+        <f>F6+G5</f>
         <v>0</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6">
-        <f t="shared" si="0"/>
+        <f>H6+I5</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7">
-        <f t="shared" si="0"/>
+        <f>B7+C6</f>
         <v>0</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7">
-        <f t="shared" si="0"/>
+        <f>D7+E6</f>
         <v>0</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7">
-        <f t="shared" si="0"/>
+        <f>F7+G6</f>
         <v>0</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7">
-        <f t="shared" si="0"/>
+        <f>H7+I6</f>
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="C8:I10" si="0">B8+C7</f>
         <v>0</v>
       </c>
       <c r="D8" s="1"/>
@@ -1533,7 +1589,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9">
@@ -1556,9 +1612,39 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F10" s="1"/>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H10" s="1"/>
+      <c r="I10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G13" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1570,10 +1656,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4308AF0-1A06-034F-BAB5-7865B37F1195}">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView zoomScale="200" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1686,61 +1772,61 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6">
-        <f t="shared" ref="C6:I9" si="0">B6+C5</f>
+        <f>B6+C5</f>
         <v>0</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6">
-        <f t="shared" si="0"/>
+        <f>D6+E5</f>
         <v>0</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6">
-        <f t="shared" si="0"/>
+        <f>F6+G5</f>
         <v>0</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6">
-        <f t="shared" si="0"/>
+        <f>H6+I5</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7">
-        <f t="shared" si="0"/>
+        <f>B7+C6</f>
         <v>0</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7">
-        <f t="shared" si="0"/>
+        <f>D7+E6</f>
         <v>0</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7">
-        <f t="shared" si="0"/>
+        <f>F7+G6</f>
         <v>0</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7">
-        <f t="shared" si="0"/>
+        <f>H7+I6</f>
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="C8:I10" si="0">B8+C7</f>
         <v>0</v>
       </c>
       <c r="D8" s="1"/>
@@ -1761,7 +1847,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9">
@@ -1784,8 +1870,33 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F10" s="1"/>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H10" s="1"/>
+      <c r="I10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1798,10 +1909,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA0D11A5-335F-3F4E-B35F-D9E2B5F99B83}">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView zoomScale="200" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="A6" sqref="A6:I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1914,61 +2025,61 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6">
-        <f t="shared" ref="C6:I9" si="0">B6+C5</f>
+        <f>B6+C5</f>
         <v>0</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6">
-        <f t="shared" si="0"/>
+        <f>D6+E5</f>
         <v>0</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6">
-        <f t="shared" si="0"/>
+        <f>F6+G5</f>
         <v>0</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6">
-        <f t="shared" si="0"/>
+        <f>H6+I5</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7">
-        <f t="shared" si="0"/>
+        <f>B7+C6</f>
         <v>0</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7">
-        <f t="shared" si="0"/>
+        <f>D7+E6</f>
         <v>0</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7">
-        <f t="shared" si="0"/>
+        <f>F7+G6</f>
         <v>0</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7">
-        <f t="shared" si="0"/>
+        <f>H7+I6</f>
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="C8:I10" si="0">B8+C7</f>
         <v>0</v>
       </c>
       <c r="D8" s="1"/>
@@ -1989,7 +2100,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9">
@@ -2012,8 +2123,33 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F10" s="1"/>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H10" s="1"/>
+      <c r="I10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2026,10 +2162,10 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94C38E3E-E40E-374A-9FD1-19FB7B86EBCE}">
   <sheetPr codeName="Sheet6"/>
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView zoomScale="200" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="A6" sqref="A6:I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2142,61 +2278,61 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6">
-        <f t="shared" ref="C6:I9" si="0">B6+C5</f>
+        <f>B6+C5</f>
         <v>0</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6">
-        <f t="shared" si="0"/>
+        <f>D6+E5</f>
         <v>0</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6">
-        <f t="shared" si="0"/>
+        <f>F6+G5</f>
         <v>0</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6">
-        <f t="shared" si="0"/>
+        <f>H6+I5</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7">
-        <f t="shared" si="0"/>
+        <f>B7+C6</f>
         <v>0</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7">
-        <f t="shared" si="0"/>
+        <f>D7+E6</f>
         <v>0</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7">
-        <f t="shared" si="0"/>
+        <f>F7+G6</f>
         <v>0</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7">
-        <f t="shared" si="0"/>
+        <f>H7+I6</f>
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="C8:I10" si="0">B8+C7</f>
         <v>0</v>
       </c>
       <c r="D8" s="1"/>
@@ -2217,7 +2353,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9">
@@ -2240,8 +2376,33 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F10" s="1"/>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H10" s="1"/>
+      <c r="I10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2254,10 +2415,10 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3114B01-EB1E-5146-A8A1-6B16EB680B75}">
   <sheetPr codeName="Sheet7"/>
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView zoomScale="200" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="A6" sqref="A6:I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2370,61 +2531,61 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6">
-        <f t="shared" ref="C6:I9" si="0">B6+C5</f>
+        <f>B6+C5</f>
         <v>0</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6">
-        <f t="shared" si="0"/>
+        <f>D6+E5</f>
         <v>0</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6">
-        <f t="shared" si="0"/>
+        <f>F6+G5</f>
         <v>0</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6">
-        <f t="shared" si="0"/>
+        <f>H6+I5</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7">
-        <f t="shared" si="0"/>
+        <f>B7+C6</f>
         <v>0</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7">
-        <f t="shared" si="0"/>
+        <f>D7+E6</f>
         <v>0</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7">
-        <f t="shared" si="0"/>
+        <f>F7+G6</f>
         <v>0</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7">
-        <f t="shared" si="0"/>
+        <f>H7+I6</f>
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="C8:I10" si="0">B8+C7</f>
         <v>0</v>
       </c>
       <c r="D8" s="1"/>
@@ -2445,7 +2606,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9">
@@ -2468,8 +2629,33 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F10" s="1"/>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H10" s="1"/>
+      <c r="I10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2482,10 +2668,10 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60565FAB-46A9-0B41-A1F0-D6DBCAC78957}">
   <sheetPr codeName="Sheet8"/>
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView zoomScale="200" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="A6" sqref="A6:I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2598,61 +2784,61 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6">
-        <f t="shared" ref="C6:I9" si="0">B6+C5</f>
+        <f>B6+C5</f>
         <v>0</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6">
-        <f t="shared" si="0"/>
+        <f>D6+E5</f>
         <v>0</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6">
-        <f t="shared" si="0"/>
+        <f>F6+G5</f>
         <v>0</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6">
-        <f t="shared" si="0"/>
+        <f>H6+I5</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7">
-        <f t="shared" si="0"/>
+        <f>B7+C6</f>
         <v>0</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7">
-        <f t="shared" si="0"/>
+        <f>D7+E6</f>
         <v>0</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7">
-        <f t="shared" si="0"/>
+        <f>F7+G6</f>
         <v>0</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7">
-        <f t="shared" si="0"/>
+        <f>H7+I6</f>
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="C8:I10" si="0">B8+C7</f>
         <v>0</v>
       </c>
       <c r="D8" s="1"/>
@@ -2673,7 +2859,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9">
@@ -2696,8 +2882,33 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F10" s="1"/>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H10" s="1"/>
+      <c r="I10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2710,10 +2921,10 @@
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E499E2B6-3917-6742-9CC8-5F507CE63656}">
   <sheetPr codeName="Sheet9"/>
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView zoomScale="200" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="A6" sqref="A6:I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2826,61 +3037,61 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6">
-        <f t="shared" ref="C6:I9" si="0">B6+C5</f>
+        <f>B6+C5</f>
         <v>0</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6">
-        <f t="shared" si="0"/>
+        <f>D6+E5</f>
         <v>0</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6">
-        <f t="shared" si="0"/>
+        <f>F6+G5</f>
         <v>0</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6">
-        <f t="shared" si="0"/>
+        <f>H6+I5</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7">
-        <f t="shared" si="0"/>
+        <f>B7+C6</f>
         <v>0</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7">
-        <f t="shared" si="0"/>
+        <f>D7+E6</f>
         <v>0</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7">
-        <f t="shared" si="0"/>
+        <f>F7+G6</f>
         <v>0</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7">
-        <f t="shared" si="0"/>
+        <f>H7+I6</f>
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="C8:I10" si="0">B8+C7</f>
         <v>0</v>
       </c>
       <c r="D8" s="1"/>
@@ -2901,7 +3112,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9">
@@ -2924,8 +3135,33 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F10" s="1"/>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H10" s="1"/>
+      <c r="I10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2938,10 +3174,10 @@
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED1EECEB-9AE6-B042-9577-6D8E66A878BB}">
   <sheetPr codeName="Sheet10"/>
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView zoomScale="200" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="A6" sqref="A6:I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3054,61 +3290,61 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6">
-        <f t="shared" ref="C6:I9" si="0">B6+C5</f>
+        <f>B6+C5</f>
         <v>0</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6">
-        <f t="shared" si="0"/>
+        <f>D6+E5</f>
         <v>0</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6">
-        <f t="shared" si="0"/>
+        <f>F6+G5</f>
         <v>0</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6">
-        <f t="shared" si="0"/>
+        <f>H6+I5</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7">
-        <f t="shared" si="0"/>
+        <f>B7+C6</f>
         <v>0</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7">
-        <f t="shared" si="0"/>
+        <f>D7+E6</f>
         <v>0</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7">
-        <f t="shared" si="0"/>
+        <f>F7+G6</f>
         <v>0</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7">
-        <f t="shared" si="0"/>
+        <f>H7+I6</f>
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="C8:I10" si="0">B8+C7</f>
         <v>0</v>
       </c>
       <c r="D8" s="1"/>
@@ -3129,7 +3365,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9">
@@ -3152,8 +3388,33 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F10" s="1"/>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H10" s="1"/>
+      <c r="I10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>